<commit_message>
Simplify baseline ride code
</commit_message>
<xml_diff>
--- a/Reproducibility Package/documentation/rider-audits/baseline-study/codebooks/ride.xlsx
+++ b/Reproducibility Package/documentation/rider-audits/baseline-study/codebooks/ride.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb501238\Documents\GitHub\rio_vagao_rosa\documentation\rider-audits\baseline-study\codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb501238\Documents\GitHub\rio-safe-space\Reproducibility Package\documentation\rider-audits\baseline-study\codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716A28C7-B0F9-460A-BE12-EE4F8B113F2F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F842301-7AAE-47C3-B34C-30C27E2AF6FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="124">
   <si>
     <t>name</t>
   </si>
@@ -364,6 +364,36 @@
   </si>
   <si>
     <t>Ride - time task started (GMT)</t>
+  </si>
+  <si>
+    <t>submitted</t>
+  </si>
+  <si>
+    <t>spectranslated</t>
+  </si>
+  <si>
+    <t>obs_uid</t>
+  </si>
+  <si>
+    <t>employment</t>
+  </si>
+  <si>
+    <t>earnings</t>
+  </si>
+  <si>
+    <t>campaign_id</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>marital_status</t>
   </si>
 </sst>
 </file>
@@ -712,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1720,6 +1750,56 @@
       </c>
       <c r="E40" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="E41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="E42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="E43" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="E44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="E45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="E46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="E47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="E48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5">
+      <c r="E49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5">
+      <c r="E50" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>